<commit_message>
And more requested fixes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
+++ b/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">In 2011–12, 4.9 per cent of Australian adults aged 25 and over were estimated to have had Type 2 diabetes—currently satisfying the 5.0 per cent proxy benchmark.</t>
+    <t xml:space="preserve">In 2011–12, 4.9 per cent of Australian adults aged 25 and over were estimated to have Type 2 diabetes—currently satisfying the 5.0 per cent proxy benchmark.</t>
   </si>
   <si>
     <t xml:space="preserve">Nationally, men (6.3 per cent) were more likely than women (3.6 per cent) to have Type 2 diabetes. Indigenous Australians were over three times as likely to have Type 2 diabetes as non- Indigenous Australians— 14.8 per cent and 4.8 per cent of persons aged 25 and over, respectively.</t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Influences</t>
   </si>
   <si>
-    <t xml:space="preserve">The prevalence of Type 2 diabetes is increased through hereditary factors and lifestyle risk factors including poor diet, insufficient physical activity and being overweight or obese.</t>
+    <t xml:space="preserve">The risk of Type 2 diabetes is increased through hereditary factors and lifestyle risk factors including poor diet, insufficient physical activity and being overweight or obese.</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -133,7 +133,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,87 +156,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -252,7 +171,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,74 +180,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -346,7 +208,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -370,55 +232,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,124 +242,48 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -758,7 +496,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -800,7 +538,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -814,7 +552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -842,7 +580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
men/women->males/females in health diabetes text.
</commit_message>
<xml_diff>
--- a/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
+++ b/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
@@ -98,7 +98,7 @@
     <t xml:space="preserve">In 2011–12, 4.9 per cent of Australian adults aged 25 and over were estimated to have Type 2 diabetes—currently satisfying the 5.0 per cent proxy benchmark.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nationally, men (6.3 per cent) were more likely than women (3.6 per cent) to have Type 2 diabetes. Indigenous Australians were over three times as likely to have Type 2 diabetes as non- Indigenous Australians— 14.8 per cent and 4.8 per cent of persons aged 25 and over, respectively.</t>
+    <t xml:space="preserve">Nationally, males (6.3 per cent) were more likely than females (3.6 per cent) to have Type 2 diabetes. Indigenous Australians were over three times as likely to have Type 2 diabetes as non- Indigenous Australians— 14.8 per cent and 4.8 per cent of persons aged 25 and over, respectively.</t>
   </si>
   <si>
     <t xml:space="preserve">Influences</t>
@@ -496,7 +496,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,7 +546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
         <v>25</v>

</xml_diff>